<commit_message>
adding uncertainty variation pf calculation
</commit_message>
<xml_diff>
--- a/Hardware/Reading/TukeyHSD_result_relative_error.xlsx
+++ b/Hardware/Reading/TukeyHSD_result_relative_error.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -488,10 +488,10 @@
         <v>0.03567018831277641</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0144401353391809</v>
+        <v>0.01033416546889408</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05690024128637192</v>
+        <v>0.06100621115665873</v>
       </c>
       <c r="G2" t="n">
         <v>6.483983340770079</v>
@@ -518,10 +518,10 @@
         <v>0.2694406281200616</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2482385524824858</v>
+        <v>0.244137993531281</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2906427037576375</v>
+        <v>0.2947432627088423</v>
       </c>
       <c r="G3" t="n">
         <v>49.04246251581599</v>
@@ -548,10 +548,10 @@
         <v>0.103729687185124</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0825506973168858</v>
+        <v>0.07845460323788132</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1249086770533623</v>
+        <v>0.1290047711323667</v>
       </c>
       <c r="G4" t="n">
         <v>18.90102652945543</v>
@@ -578,10 +578,10 @@
         <v>0.2104022417603486</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1892232518921104</v>
+        <v>0.1851271578131059</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2315812316285868</v>
+        <v>0.2356773257075913</v>
       </c>
       <c r="G5" t="n">
         <v>38.33828541555231</v>
@@ -608,10 +608,10 @@
         <v>0.2337704398072852</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2139576424545507</v>
+        <v>0.2101257750033669</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2535832371600197</v>
+        <v>0.2574151046112035</v>
       </c>
       <c r="G6" t="n">
         <v>45.53353440443567</v>
@@ -638,10 +638,10 @@
         <v>0.06805949887234762</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04827140802360795</v>
+        <v>0.04444431890063329</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08784758972108729</v>
+        <v>0.09167467884406195</v>
       </c>
       <c r="G7" t="n">
         <v>13.27310156244343</v>
@@ -668,10 +668,10 @@
         <v>0.1747320534475722</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1549439625988325</v>
+        <v>0.1511168734758578</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1945201442963118</v>
+        <v>0.1983472334192865</v>
       </c>
       <c r="G8" t="n">
         <v>34.07659959374484</v>
@@ -698,10 +698,10 @@
         <v>0.1657109409349376</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1459528691282609</v>
+        <v>0.1421315857977823</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1854690127416143</v>
+        <v>0.1892902960720929</v>
       </c>
       <c r="G9" t="n">
         <v>32.36638456443772</v>
@@ -728,10 +728,10 @@
         <v>0.05903838635971304</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03928031455303636</v>
+        <v>0.03545903122255778</v>
       </c>
       <c r="F10" t="n">
-        <v>0.07879645816638971</v>
+        <v>0.08261774149686829</v>
       </c>
       <c r="G10" t="n">
         <v>11.53127914307468</v>
@@ -758,10 +758,10 @@
         <v>0.1066725545752246</v>
       </c>
       <c r="E11" t="n">
-        <v>0.08693925778996234</v>
+        <v>0.08312276603921226</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1264058513604868</v>
+        <v>0.1302223431112369</v>
       </c>
       <c r="G11" t="n">
         <v>20.86126375611083</v>
@@ -771,6 +771,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>